<commit_message>
refatora funções de extração no scraping.py para melhorar a legibilidade e evitar duplicação de links
</commit_message>
<xml_diff>
--- a/problemas.xlsx
+++ b/problemas.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -467,6 +467,23 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Registrar elogio aos servidores</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>https://www.ms.gov.br/comunicacao-e-transparencia/teste-4189</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Seção 'Outras Informações' não encontrada</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
refatora função de extração 'Quem pode utilizar' para evitar duplicação de parágrafos e melhora a legibilidade
</commit_message>
<xml_diff>
--- a/problemas.xlsx
+++ b/problemas.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -467,23 +467,6 @@
         </is>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Registrar elogio aos servidores</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>https://www.ms.gov.br/comunicacao-e-transparencia/teste-4189</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Seção 'Outras Informações' não encontrada</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
refatora função de extração de texto para evitar duplicação e melhorar a legibilidade
</commit_message>
<xml_diff>
--- a/problemas.xlsx
+++ b/problemas.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,15 +453,253 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Serviços de transporte</t>
+          <t>Acessar agência virtual</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>https://www.ms.gov.br/educacao-e-pesquisa/servicos-de-transporte111</t>
+          <t>https://www.ms.gov.br/energia/agencia-virtual22</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
+        <is>
+          <t>Seção 'O que é este serviço' não encontrada</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Acessar agência virtual</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>https://www.ms.gov.br/energia/agencia-virtual22</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Seção 'Exigências' não encontrada</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Acessar agência virtual</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>https://www.ms.gov.br/energia/agencia-virtual22</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Seção 'Quem pode utilizar' não encontrada</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Acessar agência virtual</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>https://www.ms.gov.br/energia/agencia-virtual22</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Seção 'Prazos' não encontrada</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Acessar agência virtual</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>https://www.ms.gov.br/energia/agencia-virtual22</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Seção 'Custos' não encontrada</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Acessar dados do portal da transparência</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>https://www.ms.gov.br/comunicacao-e-transparencia/acessar-dados-do-portal-da-transparencia171</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Seção 'Outras Informações' não encontrada</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Acessar agência virtual</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>https://www.ms.gov.br/energia/agencia-virtual22</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Seção 'Etapas' não encontrada</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Acessar agência virtual</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>https://www.ms.gov.br/energia/agencia-virtual22</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Seção 'Outras Informações' não encontrada</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Acessar gratuitamente programas da TV educativa (Portal da Educativa)</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>https://www.ms.gov.br/educacao-e-pesquisa/acessar-gratuitamente-programas-da-tv-educativa-portal-da-educativa175</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Seção 'O que é este serviço' não encontrada</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Acessar gratuitamente programas da TV educativa (Portal da Educativa)</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>https://www.ms.gov.br/educacao-e-pesquisa/acessar-gratuitamente-programas-da-tv-educativa-portal-da-educativa175</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Seção 'Exigências' não encontrada</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Acessar gratuitamente programas da TV educativa (Portal da Educativa)</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>https://www.ms.gov.br/educacao-e-pesquisa/acessar-gratuitamente-programas-da-tv-educativa-portal-da-educativa175</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Seção 'Quem pode utilizar' não encontrada</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Acessar gratuitamente programas da TV educativa (Portal da Educativa)</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>https://www.ms.gov.br/educacao-e-pesquisa/acessar-gratuitamente-programas-da-tv-educativa-portal-da-educativa175</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Seção 'Prazos' não encontrada</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Acessar gratuitamente programas da TV educativa (Portal da Educativa)</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>https://www.ms.gov.br/educacao-e-pesquisa/acessar-gratuitamente-programas-da-tv-educativa-portal-da-educativa175</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Seção 'Custos' não encontrada</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Acessar gratuitamente programas da TV educativa (Portal da Educativa)</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>https://www.ms.gov.br/educacao-e-pesquisa/acessar-gratuitamente-programas-da-tv-educativa-portal-da-educativa175</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Seção 'Etapas' não encontrada</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Acessar gratuitamente programas da TV educativa (Portal da Educativa)</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>https://www.ms.gov.br/educacao-e-pesquisa/acessar-gratuitamente-programas-da-tv-educativa-portal-da-educativa175</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
         <is>
           <t>Seção 'Outras Informações' não encontrada</t>
         </is>

</xml_diff>